<commit_message>
secure link and dash board classes added
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10968" windowHeight="4260" firstSheet="14" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12228" windowHeight="4260" firstSheet="14" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
   <si>
     <t>Username</t>
   </si>
@@ -501,6 +501,12 @@
   </si>
   <si>
     <t>This is Accept comment</t>
+  </si>
+  <si>
+    <t>Search WF:The Task user accept the document</t>
+  </si>
+  <si>
+    <t>Search WF:Third User Ram Did EndWF</t>
   </si>
 </sst>
 </file>
@@ -1467,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1596,6 +1602,14 @@
     <row r="7" spans="1:8">
       <c r="B7" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
64bit latest merged codes
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisha.r\eclipse-workspace\CVS_Auto_2024_B2_64Bit\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15150" windowHeight="2955" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8415" windowHeight="5550" firstSheet="16" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
@@ -26,12 +31,10 @@
     <sheet name="Security" sheetId="39" r:id="rId17"/>
     <sheet name="DocumentVersion" sheetId="40" r:id="rId18"/>
     <sheet name="MyPreferences" sheetId="41" r:id="rId19"/>
-    <sheet name="SpecialCharFiles" sheetId="42" r:id="rId20"/>
-    <sheet name="Custom Columns" sheetId="43" r:id="rId21"/>
-    <sheet name="Templates" sheetId="44" r:id="rId22"/>
+    <sheet name="Custom Columns" sheetId="43" r:id="rId20"/>
+    <sheet name="Templates" sheetId="44" r:id="rId21"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F7"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="193">
   <si>
     <t>Username</t>
   </si>
@@ -305,66 +308,6 @@
     <t>ram</t>
   </si>
   <si>
-    <t>ReportName</t>
-  </si>
-  <si>
-    <t>Percentage Character filename</t>
-  </si>
-  <si>
-    <t>Tile Character filename</t>
-  </si>
-  <si>
-    <t>Attherate Character filename</t>
-  </si>
-  <si>
-    <t>Hash Character filename</t>
-  </si>
-  <si>
-    <t>Dollar Character filename</t>
-  </si>
-  <si>
-    <t>Plus Character filename</t>
-  </si>
-  <si>
-    <t>Caret Character filename</t>
-  </si>
-  <si>
-    <t>Equals Character filename</t>
-  </si>
-  <si>
-    <t>SingleQuote Character filename</t>
-  </si>
-  <si>
-    <t>Comma Character filename</t>
-  </si>
-  <si>
-    <t>Exclamatory Character filename</t>
-  </si>
-  <si>
-    <t>Hyphen Character filename</t>
-  </si>
-  <si>
-    <t>RoundBrackets Character filename</t>
-  </si>
-  <si>
-    <t>Accent Character filename</t>
-  </si>
-  <si>
-    <t>Ampersant Character filename</t>
-  </si>
-  <si>
-    <t>Underscore Character filename</t>
-  </si>
-  <si>
-    <t>Flowerbracket Character filename</t>
-  </si>
-  <si>
-    <t>Squarebracket Character filename</t>
-  </si>
-  <si>
-    <t>(SemiColon) Character filename All validation</t>
-  </si>
-  <si>
     <t>New_Templates1</t>
   </si>
   <si>
@@ -460,9 +403,6 @@
     <t>Workflow Accepted Successfully</t>
   </si>
   <si>
-    <t xml:space="preserve">Batch Indexing </t>
-  </si>
-  <si>
     <t>This folder is created for Batch Indexing</t>
   </si>
   <si>
@@ -603,36 +543,18 @@
     <t>Create document</t>
   </si>
   <si>
-    <t>admin2</t>
-  </si>
-  <si>
-    <t>Admin1</t>
-  </si>
-  <si>
     <t>Document has been Updated Successfully</t>
   </si>
   <si>
-    <t>Document Version Test</t>
-  </si>
-  <si>
     <t>Version test Report name Updated</t>
   </si>
   <si>
-    <t>Testing Document</t>
-  </si>
-  <si>
-    <t>Student Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enter Comment </t>
   </si>
   <si>
     <t>Login Roomname</t>
   </si>
   <si>
-    <t>EWA Url</t>
-  </si>
-  <si>
     <t>Load More count</t>
   </si>
   <si>
@@ -666,14 +588,62 @@
     <t>Report /Document Name</t>
   </si>
   <si>
-    <t>cvnamed</t>
+    <t xml:space="preserve">Stamp </t>
+  </si>
+  <si>
+    <t>SignHereStamps</t>
+  </si>
+  <si>
+    <t>Dynamic stamps</t>
+  </si>
+  <si>
+    <t>Standard Stamps</t>
+  </si>
+  <si>
+    <t>Custom stamps</t>
+  </si>
+  <si>
+    <t>SIDBI URL</t>
+  </si>
+  <si>
+    <t>Static OTP</t>
+  </si>
+  <si>
+    <t>TestServer_2024B264bit.CV2024B2_64bitDB</t>
+  </si>
+  <si>
+    <t>http://10.4.10.21:8080/CVWeb/cvLgn</t>
+  </si>
+  <si>
+    <t>Oi5FQS</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BatchIndexing </t>
+  </si>
+  <si>
+    <t>cvadmin</t>
+  </si>
+  <si>
+    <t>ECGroup</t>
+  </si>
+  <si>
+    <t>Automation Custom Stamp</t>
+  </si>
+  <si>
+    <t>Verify Register Custom Stamp Lead View</t>
+  </si>
+  <si>
+    <t>Verify Register Custom Stamp Advanced View</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,12 +687,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -732,18 +696,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -835,7 +787,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -860,21 +812,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -891,18 +839,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1233,12 +1180,12 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1336,16 +1283,16 @@
         <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1423,10 +1370,10 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
         <v>49</v>
@@ -1457,7 +1404,7 @@
     </row>
     <row r="4" spans="1:8" ht="60">
       <c r="A4" s="5" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
@@ -1474,13 +1421,13 @@
     </row>
     <row r="5" spans="1:8" ht="60">
       <c r="A5" s="5" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1488,20 +1435,20 @@
         <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1511,41 +1458,45 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="180">
       <c r="A1" s="5" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1553,18 +1504,35 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="28" customFormat="1">
+      <c r="A6" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1574,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1589,73 +1557,78 @@
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="24" t="s">
+      <c r="C1" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="27">
-        <v>40</v>
-      </c>
-      <c r="F2" s="27">
+      <c r="C2" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="7">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
-        <v>162</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="27">
-        <v>150</v>
-      </c>
-      <c r="F3" s="27">
+      <c r="E3" s="7">
+        <v>60</v>
+      </c>
+      <c r="F3" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
-        <v>183</v>
-      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="7"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1677,7 +1650,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1688,31 +1661,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>195</v>
+      <c r="C1" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>135</v>
+        <v>187</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1734,7 +1707,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1747,57 +1720,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>133</v>
+      <c r="E1" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>183</v>
+        <v>48</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>117</v>
+        <v>96</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>97</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="7"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="6"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="8" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1822,7 +1795,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1833,19 +1806,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="E1" s="22" t="s">
+      <c r="C1" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1853,29 +1826,29 @@
       <c r="A2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>117</v>
+        <v>132</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6"/>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -1883,10 +1856,10 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="E4" s="6"/>
     </row>
@@ -1894,10 +1867,10 @@
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -1905,10 +1878,10 @@
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -1916,10 +1889,10 @@
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="E7" s="6"/>
     </row>
@@ -1927,18 +1900,18 @@
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="19" t="s">
-        <v>116</v>
+      <c r="C9" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1946,8 +1919,8 @@
     <row r="10" spans="1:5">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="19" t="s">
-        <v>118</v>
+      <c r="C10" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1955,8 +1928,8 @@
     <row r="11" spans="1:5">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="19" t="s">
-        <v>150</v>
+      <c r="C11" s="17" t="s">
+        <v>129</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1964,8 +1937,8 @@
     <row r="12" spans="1:5">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="19" t="s">
-        <v>152</v>
+      <c r="C12" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1991,7 +1964,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2001,36 +1974,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="27" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>4</v>
+      <c r="B2" s="22" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="19" t="s">
-        <v>203</v>
+      <c r="A5" s="17" t="s">
+        <v>189</v>
       </c>
       <c r="B5" s="6"/>
     </row>
@@ -2040,7 +2013,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" display="syntax@10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2051,7 +2024,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2060,18 +2033,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="22" t="s">
-        <v>199</v>
+      <c r="A1" s="20" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>185</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -2080,8 +2053,8 @@
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="19" t="s">
-        <v>186</v>
+      <c r="A5" s="17" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -2094,114 +2067,129 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="22" t="s">
-        <v>200</v>
+      <c r="A1" s="20" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="13" t="s">
-        <v>187</v>
+      <c r="A2" s="11" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="11" t="s">
-        <v>105</v>
+      <c r="A3" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
-        <v>106</v>
+      <c r="A4" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="7" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="14" t="s">
-        <v>110</v>
+      <c r="A6" s="12" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="15" t="s">
-        <v>111</v>
+      <c r="A7" s="13" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="16" t="s">
-        <v>112</v>
+      <c r="A8" s="14" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="17">
+      <c r="A9" s="15">
         <v>78304</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="17" t="s">
-        <v>113</v>
+      <c r="A11" s="15" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="17" t="s">
-        <v>104</v>
+      <c r="A12" s="15" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="18" t="s">
-        <v>114</v>
+      <c r="A13" s="16" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="18" t="s">
-        <v>115</v>
+      <c r="A15" s="16" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="18" t="s">
-        <v>137</v>
+      <c r="A16" s="16" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="18" t="s">
-        <v>111</v>
+      <c r="A17" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="18" t="s">
-        <v>161</v>
+      <c r="A18" s="16" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="12" t="s">
-        <v>109</v>
+      <c r="A19" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="6"/>
+      <c r="A20" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2253,10 +2241,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>168</v>
+        <v>142</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2264,22 +2252,22 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="C9" s="21" t="s">
-        <v>164</v>
+      <c r="C9" s="19" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2290,131 +2278,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2423,63 +2290,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="22" t="s">
-        <v>151</v>
+      <c r="A1" s="20" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="6"/>
+      <c r="A4" s="17" t="s">
+        <v>163</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2489,43 +2328,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="32" t="s">
-        <v>202</v>
+      <c r="A1" s="29" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="10" t="s">
-        <v>104</v>
+      <c r="A2" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="11" t="s">
-        <v>105</v>
+      <c r="A3" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
-        <v>106</v>
+      <c r="A4" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="11" t="s">
-        <v>138</v>
+      <c r="A5" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="11" t="s">
-        <v>107</v>
+      <c r="A6" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="11" t="s">
-        <v>108</v>
+      <c r="A7" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="14" t="s">
-        <v>110</v>
+      <c r="A8" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -2551,55 +2390,55 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes has been done
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15552" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="2070" firstSheet="19" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Templates" sheetId="44" r:id="rId22"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J8"/>
+  <oleSize ref="A1:K4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="216">
   <si>
     <t>Username</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>syntax@10</t>
-  </si>
-  <si>
-    <t>CVWin19Server.Win2019_TestRoom</t>
   </si>
   <si>
     <t>vid</t>
@@ -254,9 +251,6 @@
     <t>content</t>
   </si>
   <si>
-    <t>http://10.4.10.60:8080/CVWeb/cvLgn</t>
-  </si>
-  <si>
     <t>nisha.rahamah@computhink.in</t>
   </si>
   <si>
@@ -460,9 +454,6 @@
     <t>Workflow Accepted Successfully</t>
   </si>
   <si>
-    <t xml:space="preserve">Batch Indexing </t>
-  </si>
-  <si>
     <t>This folder is created for Batch Indexing</t>
   </si>
   <si>
@@ -603,36 +594,21 @@
     <t>Create document</t>
   </si>
   <si>
-    <t>admin2</t>
-  </si>
-  <si>
     <t>Admin1</t>
   </si>
   <si>
     <t>Document has been Updated Successfully</t>
   </si>
   <si>
-    <t>Document Version Test</t>
-  </si>
-  <si>
     <t>Version test Report name Updated</t>
   </si>
   <si>
-    <t>Testing Document</t>
-  </si>
-  <si>
-    <t>Student Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enter Comment </t>
   </si>
   <si>
     <t>Login Roomname</t>
   </si>
   <si>
-    <t>EWA Url</t>
-  </si>
-  <si>
     <t>Load More count</t>
   </si>
   <si>
@@ -666,9 +642,6 @@
     <t>Report /Document Name</t>
   </si>
   <si>
-    <t>cvnamed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stamp </t>
   </si>
   <si>
@@ -694,13 +667,49 @@
   </si>
   <si>
     <t>Robert</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Static OTP</t>
+  </si>
+  <si>
+    <t>TestServer_2024B264bit.vw56demo</t>
+  </si>
+  <si>
+    <t>http://10.4.10.21:8080/CVWeb/cvLgn</t>
+  </si>
+  <si>
+    <t>Oi5FQS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BatchIndexing </t>
+  </si>
+  <si>
+    <t>Alkas</t>
+  </si>
+  <si>
+    <t>cvadmin</t>
+  </si>
+  <si>
+    <t>ECGroup</t>
+  </si>
+  <si>
+    <t>Automation Custom Stamp</t>
+  </si>
+  <si>
+    <t>Verify Register Custom Stamp Lead View</t>
+  </si>
+  <si>
+    <t>Verify Register Custom Stamp Advanced View</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -759,18 +768,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -862,7 +859,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -887,7 +884,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -918,21 +914,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1211,15 +1203,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1235,49 +1227,49 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -1285,7 +1277,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1293,7 +1285,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -1320,93 +1312,93 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1427,73 +1419,73 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="35.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1505,59 +1497,59 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="60">
+      <c r="A4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="57.6">
-      <c r="A4" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60">
+      <c r="A5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
         <v>122</v>
       </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="57.6">
-      <c r="A5" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>124</v>
-      </c>
-      <c r="C5" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1573,39 +1565,39 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="158.4">
+    <row r="1" spans="1:5" ht="180">
       <c r="A1" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
         <v>142</v>
-      </c>
-      <c r="E3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1613,35 +1605,35 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" t="s">
         <v>143</v>
-      </c>
-      <c r="E4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" t="s">
         <v>144</v>
       </c>
-      <c r="E5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="33" customFormat="1">
-      <c r="A6" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>208</v>
+    </row>
+    <row r="6" spans="1:5" s="29" customFormat="1">
+      <c r="A6" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1651,99 +1643,95 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="21" style="6" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="24" t="s">
+      <c r="C1" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1">
+      <c r="A2" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="27">
-        <v>40</v>
-      </c>
-      <c r="F2" s="27">
+      <c r="C2" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="7">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1">
       <c r="A3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="27">
-        <v>150</v>
-      </c>
-      <c r="F3" s="27">
+        <v>179</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7">
+        <v>60</v>
+      </c>
+      <c r="F3" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" s="6" customFormat="1"/>
+    <row r="5" spans="1:7" s="6" customFormat="1"/>
+    <row r="6" spans="1:7" s="6" customFormat="1"/>
+    <row r="7" spans="1:7" s="6" customFormat="1"/>
+    <row r="8" spans="1:7" s="6" customFormat="1"/>
+    <row r="9" spans="1:7" s="6" customFormat="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1754,50 +1742,47 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="1" max="1" width="17" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="C1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="6" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>135</v>
+        <v>209</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1811,79 +1796,69 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
-    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="C1" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="7"/>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1">
+      <c r="A3" s="32"/>
       <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+        <v>6</v>
+      </c>
       <c r="E3" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1">
+      <c r="A4" s="32"/>
       <c r="E4" s="8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="6" customFormat="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1899,60 +1874,60 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
-    <col min="4" max="4" width="37.88671875" customWidth="1"/>
-    <col min="5" max="5" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>23</v>
+      <c r="C1" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>117</v>
+        <v>150</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6"/>
-      <c r="B3" s="30" t="s">
-        <v>7</v>
+      <c r="B3" s="27" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -1960,10 +1935,10 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E4" s="6"/>
     </row>
@@ -1971,10 +1946,10 @@
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -1982,10 +1957,10 @@
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -1993,10 +1968,10 @@
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E7" s="6"/>
     </row>
@@ -2004,18 +1979,18 @@
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="19" t="s">
-        <v>116</v>
+      <c r="C9" s="18" t="s">
+        <v>114</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -2023,8 +1998,8 @@
     <row r="10" spans="1:5">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="19" t="s">
-        <v>118</v>
+      <c r="C10" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -2032,8 +2007,8 @@
     <row r="11" spans="1:5">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="19" t="s">
-        <v>150</v>
+      <c r="C11" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -2041,8 +2016,8 @@
     <row r="12" spans="1:5">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="19" t="s">
-        <v>152</v>
+      <c r="C12" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -2056,8 +2031,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2068,56 +2043,51 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:2" s="6" customFormat="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B1" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1">
+      <c r="A2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1">
       <c r="A3" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="6" customFormat="1">
       <c r="A4" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-    </row>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="6" customFormat="1">
+      <c r="A5" s="18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="6" customFormat="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" display="syntax@10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2128,42 +2098,41 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="22" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:1" s="6" customFormat="1">
+      <c r="A1" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="6" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="6" customFormat="1">
       <c r="A3" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="6" customFormat="1">
       <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="6"/>
-    </row>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="6" customFormat="1">
+      <c r="A5" s="18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="6" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2171,115 +2140,129 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+    <row r="1" spans="1:1" s="6" customFormat="1">
+      <c r="A1" s="21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="6" customFormat="1">
+      <c r="A2" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="6" customFormat="1">
+      <c r="A3" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="6" customFormat="1">
+      <c r="A4" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="6" customFormat="1">
       <c r="A5" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="6" customFormat="1">
+      <c r="A6" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="6" customFormat="1">
+      <c r="A7" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="6" customFormat="1">
+      <c r="A8" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="15" t="s">
+    <row r="9" spans="1:1" s="6" customFormat="1">
+      <c r="A9" s="16">
+        <v>78304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="6" customFormat="1">
+      <c r="A10" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="6" customFormat="1">
+      <c r="A11" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="16" t="s">
+    <row r="12" spans="1:1" s="6" customFormat="1">
+      <c r="A12" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="6" customFormat="1">
+      <c r="A13" s="17" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="17">
-        <v>78304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="17" t="s">
+    <row r="14" spans="1:1" s="6" customFormat="1">
+      <c r="A14" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="6" customFormat="1">
+      <c r="A15" s="17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="12" t="s">
+    <row r="16" spans="1:1" s="6" customFormat="1">
+      <c r="A16" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="6" customFormat="1">
+      <c r="A17" s="17" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="6"/>
-    </row>
+    <row r="18" spans="1:1" s="6" customFormat="1">
+      <c r="A18" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="6" customFormat="1">
+      <c r="A19" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="6" customFormat="1">
+      <c r="A20" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="6" customFormat="1">
+      <c r="A21" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="6" customFormat="1">
+      <c r="A22" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="6" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2293,31 +2276,31 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2325,38 +2308,38 @@
         <v>9966881234</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="C9" s="21" t="s">
-        <v>164</v>
+      <c r="C9" s="20" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2373,109 +2356,109 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="22" t="s">
-        <v>84</v>
+      <c r="A1" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -2491,62 +2474,41 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:1" s="6" customFormat="1">
+      <c r="A1" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="6" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" s="6" customFormat="1">
       <c r="A3" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="6"/>
-    </row>
+    <row r="4" spans="1:1" s="6" customFormat="1">
+      <c r="A4" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="6" customFormat="1"/>
+    <row r="6" spans="1:1" s="6" customFormat="1"/>
+    <row r="7" spans="1:1" s="6" customFormat="1"/>
+    <row r="8" spans="1:1" s="6" customFormat="1"/>
+    <row r="9" spans="1:1" s="6" customFormat="1"/>
+    <row r="10" spans="1:1" s="6" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2556,58 +2518,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="32" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:1" s="6" customFormat="1">
+      <c r="A1" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="6" customFormat="1">
+      <c r="A2" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="6" customFormat="1">
+      <c r="A3" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="6" customFormat="1">
+      <c r="A4" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="11" t="s">
+    <row r="5" spans="1:1" s="6" customFormat="1">
+      <c r="A5" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="6" customFormat="1">
+      <c r="A6" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
+    <row r="7" spans="1:1" s="6" customFormat="1">
+      <c r="A7" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="11" t="s">
+    <row r="8" spans="1:1" s="6" customFormat="1">
+      <c r="A8" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="6"/>
-    </row>
+    <row r="9" spans="1:1" s="6" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2621,62 +2582,62 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" t="s">
         <v>178</v>
-      </c>
-      <c r="B5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2695,11 +2656,11 @@
       <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2715,13 +2676,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2729,18 +2690,18 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2748,7 +2709,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2764,33 +2725,33 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2806,26 +2767,26 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2841,17 +2802,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="4"/>
+    <col min="1" max="2" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2875,10 +2836,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2901,7 +2862,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2924,71 +2885,71 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="C4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="D6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nish r branch codes
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="2445" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15552" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Templates" sheetId="44" r:id="rId22"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E6"/>
+  <oleSize ref="A1:J8"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="213">
   <si>
     <t>Username</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>syntax@10</t>
+  </si>
+  <si>
+    <t>CVWin19Server.Win2019_TestRoom</t>
   </si>
   <si>
     <t>vid</t>
@@ -251,6 +254,9 @@
     <t>content</t>
   </si>
   <si>
+    <t>http://10.4.10.60:8080/CVWeb/cvLgn</t>
+  </si>
+  <si>
     <t>nisha.rahamah@computhink.in</t>
   </si>
   <si>
@@ -454,6 +460,9 @@
     <t>Workflow Accepted Successfully</t>
   </si>
   <si>
+    <t xml:space="preserve">Batch Indexing </t>
+  </si>
+  <si>
     <t>This folder is created for Batch Indexing</t>
   </si>
   <si>
@@ -594,21 +603,36 @@
     <t>Create document</t>
   </si>
   <si>
+    <t>admin2</t>
+  </si>
+  <si>
     <t>Admin1</t>
   </si>
   <si>
     <t>Document has been Updated Successfully</t>
   </si>
   <si>
+    <t>Document Version Test</t>
+  </si>
+  <si>
     <t>Version test Report name Updated</t>
   </si>
   <si>
+    <t>Testing Document</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Enter Comment </t>
   </si>
   <si>
     <t>Login Roomname</t>
   </si>
   <si>
+    <t>EWA Url</t>
+  </si>
+  <si>
     <t>Load More count</t>
   </si>
   <si>
@@ -642,6 +666,9 @@
     <t>Report /Document Name</t>
   </si>
   <si>
+    <t>cvnamed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stamp </t>
   </si>
   <si>
@@ -667,49 +694,13 @@
   </si>
   <si>
     <t>Robert</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Static OTP</t>
-  </si>
-  <si>
-    <t>TestServer_2024B264bit.vw56demo</t>
-  </si>
-  <si>
-    <t>http://10.4.10.21:8080/CVWeb/cvLgn</t>
-  </si>
-  <si>
-    <t>Oi5FQS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BatchIndexing </t>
-  </si>
-  <si>
-    <t>Alkas</t>
-  </si>
-  <si>
-    <t>cvadmin</t>
-  </si>
-  <si>
-    <t>ECGroup</t>
-  </si>
-  <si>
-    <t>Automation Custom Stamp</t>
-  </si>
-  <si>
-    <t>Verify Register Custom Stamp Lead View</t>
-  </si>
-  <si>
-    <t>Verify Register Custom Stamp Advanced View</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,6 +759,18 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -859,7 +862,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -884,6 +887,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -914,17 +918,21 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1203,15 +1211,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1227,49 +1235,49 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -1277,7 +1285,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1285,7 +1293,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -1312,93 +1320,93 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1419,73 +1427,73 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1497,59 +1505,59 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="60">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.6">
       <c r="A4" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6">
       <c r="A5" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1565,39 +1573,39 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="180">
+    <row r="1" spans="1:5" ht="158.4">
       <c r="A1" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1605,35 +1613,35 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="29" customFormat="1">
-      <c r="A6" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>199</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="33" customFormat="1">
+      <c r="A6" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1643,95 +1651,99 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="35" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="21" style="6" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="27">
+        <v>40</v>
+      </c>
+      <c r="F2" s="27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="27">
+        <v>150</v>
+      </c>
+      <c r="F3" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="6" customFormat="1">
-      <c r="A2" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>207</v>
-      </c>
-      <c r="E2" s="7">
-        <v>10</v>
-      </c>
-      <c r="F2" s="7">
-        <v>8</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="6" customFormat="1">
-      <c r="A3" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="7">
-        <v>60</v>
-      </c>
-      <c r="F3" s="7">
-        <v>4</v>
-      </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" s="6" customFormat="1"/>
-    <row r="5" spans="1:7" s="6" customFormat="1"/>
-    <row r="6" spans="1:7" s="6" customFormat="1"/>
-    <row r="7" spans="1:7" s="6" customFormat="1"/>
-    <row r="8" spans="1:7" s="6" customFormat="1"/>
-    <row r="9" spans="1:7" s="6" customFormat="1"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1742,47 +1754,50 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="6" customFormat="1">
+      <c r="C1" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>209</v>
+        <v>135</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1796,69 +1811,79 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="6" customFormat="1">
+      <c r="C1" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>117</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1">
-      <c r="A3" s="32"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1">
-      <c r="A4" s="32"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="6" customFormat="1"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1874,60 +1899,60 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E12"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" customWidth="1"/>
-    <col min="5" max="5" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="37.88671875" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>22</v>
+      <c r="C1" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>115</v>
+        <v>153</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6"/>
-      <c r="B3" s="27" t="s">
-        <v>6</v>
+      <c r="B3" s="30" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -1935,10 +1960,10 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E4" s="6"/>
     </row>
@@ -1946,10 +1971,10 @@
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -1957,10 +1982,10 @@
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -1968,10 +1993,10 @@
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E7" s="6"/>
     </row>
@@ -1979,18 +2004,18 @@
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="18" t="s">
-        <v>114</v>
+      <c r="C9" s="19" t="s">
+        <v>116</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1998,8 +2023,8 @@
     <row r="10" spans="1:5">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="18" t="s">
-        <v>116</v>
+      <c r="C10" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -2007,8 +2032,8 @@
     <row r="11" spans="1:5">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="18" t="s">
-        <v>147</v>
+      <c r="C11" s="19" t="s">
+        <v>150</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -2016,8 +2041,8 @@
     <row r="12" spans="1:5">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="18" t="s">
-        <v>149</v>
+      <c r="C12" s="19" t="s">
+        <v>152</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -2031,8 +2056,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2043,51 +2068,56 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1">
-      <c r="A2" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1">
+      <c r="B1" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1">
+        <v>183</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="6" customFormat="1">
-      <c r="A5" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="6" customFormat="1"/>
+        <v>149</v>
+      </c>
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="syntax@10"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2098,41 +2128,42 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="6" customFormat="1">
-      <c r="A1" s="21" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="6" customFormat="1">
+    <row r="1" spans="1:1">
+      <c r="A1" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="6" customFormat="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="6" customFormat="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="6" customFormat="1">
-      <c r="A5" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" s="6" customFormat="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2140,129 +2171,115 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="6" customFormat="1">
-      <c r="A1" s="21" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="6" customFormat="1">
-      <c r="A2" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="6" customFormat="1">
-      <c r="A3" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="6" customFormat="1">
-      <c r="A4" s="10" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="17">
+        <v>78304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="6" customFormat="1">
-      <c r="A5" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" s="6" customFormat="1">
-      <c r="A6" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" s="6" customFormat="1">
-      <c r="A7" s="14" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="6" customFormat="1">
-      <c r="A8" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="6" customFormat="1">
-      <c r="A9" s="16">
-        <v>78304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="6" customFormat="1">
-      <c r="A10" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="6" customFormat="1">
-      <c r="A11" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="6" customFormat="1">
-      <c r="A12" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="6" customFormat="1">
-      <c r="A13" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="6" customFormat="1">
-      <c r="A14" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="6" customFormat="1">
-      <c r="A15" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="6" customFormat="1">
-      <c r="A16" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="6" customFormat="1">
-      <c r="A17" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" s="6" customFormat="1">
-      <c r="A18" s="17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="6" customFormat="1">
-      <c r="A19" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="6" customFormat="1">
-      <c r="A20" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="6" customFormat="1">
-      <c r="A21" s="17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" s="6" customFormat="1">
-      <c r="A22" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" s="6" customFormat="1"/>
+    <row r="20" spans="1:1">
+      <c r="A20" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2276,31 +2293,31 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2308,38 +2325,38 @@
         <v>9966881234</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" s="21" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" s="20" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2356,109 +2373,109 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="21" t="s">
-        <v>82</v>
+      <c r="A1" s="22" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -2474,41 +2491,62 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="6" customFormat="1">
-      <c r="A1" s="21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="6" customFormat="1">
+    <row r="1" spans="1:1">
+      <c r="A1" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="6" customFormat="1">
+    <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="6" customFormat="1">
-      <c r="A4" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="6" customFormat="1"/>
-    <row r="6" spans="1:1" s="6" customFormat="1"/>
-    <row r="7" spans="1:1" s="6" customFormat="1"/>
-    <row r="8" spans="1:1" s="6" customFormat="1"/>
-    <row r="9" spans="1:1" s="6" customFormat="1"/>
-    <row r="10" spans="1:1" s="6" customFormat="1"/>
+    <row r="6" spans="1:1">
+      <c r="A6" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2519,56 +2557,57 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="6" customFormat="1">
-      <c r="A1" s="30" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="6" customFormat="1">
-      <c r="A2" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="6" customFormat="1">
-      <c r="A3" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="6" customFormat="1">
-      <c r="A4" s="7" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="6" customFormat="1">
-      <c r="A5" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" s="6" customFormat="1">
-      <c r="A6" s="7" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="6" customFormat="1">
-      <c r="A7" s="7" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="6" customFormat="1">
-      <c r="A8" s="7" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="6" customFormat="1"/>
+    <row r="8" spans="1:1">
+      <c r="A8" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2582,62 +2621,62 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" t="s">
         <v>172</v>
-      </c>
-      <c r="B2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2656,11 +2695,11 @@
       <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2676,13 +2715,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2690,18 +2729,18 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2709,7 +2748,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2725,33 +2764,33 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2767,26 +2806,26 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2802,17 +2841,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4"/>
+    <col min="1" max="2" width="9.109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2836,10 +2875,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2862,7 +2901,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2885,71 +2924,71 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="C4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="D5" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="D6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>